<commit_message>
changes in program files
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manal_\git\Team3_TechnoTribe_LMSUI_phase2_Hackathon2025\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAB61C4-BF35-46F1-A789-BBA2B057BDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFE0FB9-9A0F-41C3-A840-19B94BA2CD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
     <t>Active</t>
   </si>
   <si>
-    <t>SAPAdvanced</t>
+    <t>testsapadv</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
completed add batch scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -2,13 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="Program" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Batch" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Class" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Login" sheetId="4" r:id="rId7"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>testcase</t>
   </si>
@@ -54,16 +56,41 @@
     <t>NoOfClasses</t>
   </si>
   <si>
+    <t>validAll</t>
+  </si>
+  <si>
     <t>Inheritance-Java</t>
   </si>
   <si>
-    <t>Mathu</t>
+    <t>software development</t>
+  </si>
+  <si>
+    <t>onlyMandatory</t>
+  </si>
+  <si>
+    <t>seleniumNinja</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11.0"/>
@@ -96,12 +123,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -327,17 +357,18 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.86"/>
-    <col customWidth="1" min="2" max="2" width="14.29"/>
-    <col customWidth="1" min="3" max="3" width="19.57"/>
-    <col customWidth="1" min="4" max="4" width="14.71"/>
-    <col customWidth="1" min="5" max="6" width="8.86"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" customWidth="true" width="14.86"/>
+    <col min="2" max="2" customWidth="true" width="14.29"/>
+    <col min="3" max="3" customWidth="true" width="19.57"/>
+    <col min="4" max="4" customWidth="true" width="14.71"/>
+    <col min="5" max="6" customWidth="true" width="8.86"/>
+    <col min="7" max="26" customWidth="true" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -28369,16 +28400,17 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.86"/>
-    <col customWidth="1" min="2" max="3" width="22.43"/>
-    <col customWidth="1" min="4" max="4" width="14.43"/>
-    <col customWidth="1" min="5" max="5" width="17.86"/>
-    <col customWidth="1" min="6" max="27" width="8.71"/>
+    <col min="1" max="1" customWidth="true" width="14.86"/>
+    <col min="2" max="3" customWidth="true" width="22.43"/>
+    <col min="4" max="4" customWidth="true" width="14.43"/>
+    <col min="5" max="5" customWidth="true" width="17.86"/>
+    <col min="6" max="27" customWidth="true" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -28399,23 +28431,39 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
+      <c r="A2" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2">
         <v>2.0</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
       </c>
-      <c r="E2" s="2">
-        <v>3.0</v>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
       </c>
-    </row>
-    <row r="3" ht="14.25" customHeight="1"/>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
     <row r="4" ht="14.25" customHeight="1"/>
     <row r="5" ht="14.25" customHeight="1"/>
     <row r="6" ht="14.25" customHeight="1"/>
@@ -29431,7 +29479,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col min="1" max="26" customWidth="true" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
@@ -30452,7 +30500,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col min="1" max="26" customWidth="true" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
navigation and add batch scenarios completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -14,14 +14,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="X6Nf2l8HmhBCJALbE7r9lPHL3LOUQytr/TFM0xPY7lo="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="HmEXYPqxvpRG7s/ayNSWbAN0OTGVt72HvD0buliEC/I="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>testcase</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>BatchNamePrefix</t>
   </si>
   <si>
     <t>BatchName</t>
@@ -71,19 +74,25 @@
     <t>seleniumNinja</t>
   </si>
   <si>
-    <t>4</t>
+    <t>invalidBatchNameSuffix</t>
   </si>
   <si>
-    <t>5</t>
+    <t>invalid</t>
   </si>
   <si>
-    <t>6</t>
+    <t>invalidBatchNamePrefix</t>
   </si>
   <si>
-    <t>7</t>
+    <t>missingOneMandatory</t>
   </si>
   <si>
-    <t>3</t>
+    <t>18</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>19</t>
   </si>
 </sst>
 </file>
@@ -28400,17 +28409,17 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.86"/>
-    <col min="2" max="3" customWidth="true" width="22.43"/>
-    <col min="4" max="4" customWidth="true" width="14.43"/>
-    <col min="5" max="5" customWidth="true" width="17.86"/>
-    <col min="6" max="27" customWidth="true" width="8.71"/>
+    <col min="1" max="1" customWidth="true" width="23.86"/>
+    <col min="2" max="4" customWidth="true" width="22.43"/>
+    <col min="5" max="5" customWidth="true" width="14.43"/>
+    <col min="6" max="6" customWidth="true" width="17.86"/>
+    <col min="7" max="28" customWidth="true" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -28429,44 +28438,77 @@
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2">
         <v>2.0</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1"/>
-    <row r="5" ht="14.25" customHeight="1"/>
-    <row r="6" ht="14.25" customHeight="1"/>
     <row r="7" ht="14.25" customHeight="1"/>
     <row r="8" ht="14.25" customHeight="1"/>
     <row r="9" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
chaining works for program to batch
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>testcase</t>
   </si>
@@ -38,7 +38,7 @@
     <t>validInputData</t>
   </si>
   <si>
-    <t>testsapadv</t>
+    <t>technoTribe</t>
   </si>
   <si>
     <t>Advanced level SAP</t>
@@ -62,7 +62,7 @@
     <t>validAll</t>
   </si>
   <si>
-    <t>Inheritance-Java</t>
+    <t>chaining</t>
   </si>
   <si>
     <t>software development</t>
@@ -86,13 +86,16 @@
     <t>missingOneMandatory</t>
   </si>
   <si>
-    <t>18</t>
+    <t>technoTribej</t>
   </si>
   <si>
-    <t>15</t>
+    <t>17</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
   </si>
 </sst>
 </file>
@@ -137,10 +140,10 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -420,8 +423,8 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -28429,83 +28432,83 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <v>2.0</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>24</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <v>2.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edit scenarios for batch completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>testcase</t>
   </si>
@@ -71,7 +71,7 @@
     <t>onlyMandatory</t>
   </si>
   <si>
-    <t>seleniumNinja</t>
+    <t>techNoTribeNumpy</t>
   </si>
   <si>
     <t>invalidBatchNameSuffix</t>
@@ -86,16 +86,19 @@
     <t>missingOneMandatory</t>
   </si>
   <si>
-    <t>technoTribej</t>
+    <t>editAll</t>
   </si>
   <si>
-    <t>17</t>
+    <t>testing</t>
   </si>
   <si>
-    <t>20</t>
+    <t>editInvalid</t>
   </si>
   <si>
-    <t>21</t>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -28453,8 +28456,8 @@
         <v>13</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
+      <c r="D2" s="3">
+        <v>20.0</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>14</v>
@@ -28472,7 +28475,7 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -28512,8 +28515,25 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="3">
+        <v>12312.0</v>
+      </c>
+    </row>
     <row r="9" ht="14.25" customHeight="1"/>
     <row r="10" ht="14.25" customHeight="1"/>
     <row r="11" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
changed pagefactory initialized elements to by locators
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="21768" windowHeight="11460" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="21936" windowHeight="11460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Program" sheetId="1" r:id="rId1"/>
@@ -13,17 +13,12 @@
     <sheet name="Login" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:P40"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="HmEXYPqxvpRG7s/ayNSWbAN0OTGVt72HvD0buliEC/I="/>
-    </ext>
-  </extLst>
+  <oleSize ref="A1:O40"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>testcase</t>
   </si>
@@ -105,16 +100,86 @@
   <si>
     <t>editInvalid</t>
   </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Incorrect_DomainName</t>
+  </si>
+  <si>
+    <t>https://jan-ui-hackathon-bbfd38d67ea9.herokuapp.com/login</t>
+  </si>
+  <si>
+    <t>Misspelled_DomainName</t>
+  </si>
+  <si>
+    <t>https://feb-ui-hackathon-bbfd38d67ea9.herokUuapp.com/login</t>
+  </si>
+  <si>
+    <t>Incorrect_Protocol</t>
+  </si>
+  <si>
+    <t>httpx://feb-ui-buildathon-bbfd38d67ea99.herokuapp.com/login</t>
+  </si>
+  <si>
+    <t>Missing_Protocol</t>
+  </si>
+  <si>
+    <t>feb-ui-buildathon-bbfd38d67ea99.herokuapp.com/login</t>
+  </si>
+  <si>
+    <t>Incorrect_Endpoint</t>
+  </si>
+  <si>
+    <t>https://feb-ui-hackathon-bbfd38d67ea9.herokuapp.com/batch</t>
+  </si>
+  <si>
+    <t>Misspelled_Endpoint</t>
+  </si>
+  <si>
+    <t>https://feb-ui-hackathon-bbfd38d67ea9.herokuapp.com/logginn</t>
+  </si>
+  <si>
+    <t>Incorrect_TopLevelDomain</t>
+  </si>
+  <si>
+    <t>https://feb-ui-hackathon-bbfd38d67ea9.herokuapp.net/login</t>
+  </si>
+  <si>
+    <t>Missing_TopLevelDomain</t>
+  </si>
+  <si>
+    <t>https://feb-ui-hackathon-bbfd38d67ea9.herokuapp/</t>
+  </si>
+  <si>
+    <t>NonExistenSubDomain</t>
+  </si>
+  <si>
+    <t>https://video.feb-ui-hackathon-bbfd38d67ea9.herokuapp.com/login</t>
+  </si>
+  <si>
+    <t>InvalidCharacters</t>
+  </si>
+  <si>
+    <t>https://feb-ui-@hackathon.bbfd38d67ea9 herokuapp.com/login</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -131,6 +196,27 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -166,22 +252,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink 2" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -30563,33 +30657,112 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A1000"/>
+  <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="14.25" customHeight="1"/>
-    <row r="4" ht="14.25" customHeight="1"/>
-    <row r="5" ht="14.25" customHeight="1"/>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="2.4" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="1" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:2" ht="2.4" customHeight="1"/>
+    <row r="15" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -31575,6 +31748,15 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B10" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B3" r:id="rId6"/>
+    <hyperlink ref="B7" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>

<commit_message>
search and logout for batch completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -2,13 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="Program" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Batch" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Class" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Login" sheetId="4" r:id="rId7"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>testcase</t>
   </si>
@@ -78,7 +80,7 @@
     <t>onlyMandatory</t>
   </si>
   <si>
-    <t>techNoTribeNumpy</t>
+    <t>javaWebDriver</t>
   </si>
   <si>
     <t>invalidBatchNameSuffix</t>
@@ -220,11 +222,18 @@
   <si>
     <t>https://feb-ui-@hackathon.bbfd38d67ea9 herokuapp.com/login</t>
   </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="0"/>
   <fonts count="7">
     <font>
       <sz val="11.0"/>
@@ -545,17 +554,18 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.86"/>
-    <col customWidth="1" min="2" max="2" width="14.29"/>
-    <col customWidth="1" min="3" max="3" width="19.57"/>
-    <col customWidth="1" min="4" max="4" width="14.71"/>
-    <col customWidth="1" min="5" max="6" width="8.86"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" customWidth="true" width="14.86"/>
+    <col min="2" max="2" customWidth="true" width="14.29"/>
+    <col min="3" max="3" customWidth="true" width="19.57"/>
+    <col min="4" max="4" customWidth="true" width="14.71"/>
+    <col min="5" max="6" customWidth="true" width="8.86"/>
+    <col min="7" max="26" customWidth="true" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -28593,16 +28603,17 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.86"/>
-    <col customWidth="1" min="2" max="4" width="22.43"/>
-    <col customWidth="1" min="5" max="5" width="14.43"/>
-    <col customWidth="1" min="6" max="6" width="17.86"/>
-    <col customWidth="1" min="7" max="28" width="8.71"/>
+    <col min="1" max="1" customWidth="true" width="23.86"/>
+    <col min="2" max="4" customWidth="true" width="22.43"/>
+    <col min="5" max="5" customWidth="true" width="14.43"/>
+    <col min="6" max="6" customWidth="true" width="17.86"/>
+    <col min="7" max="28" customWidth="true" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -28651,8 +28662,8 @@
         <v>19</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="4">
-        <v>46.0</v>
+      <c r="D3" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>17</v>
@@ -29721,7 +29732,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col min="1" max="26" customWidth="true" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
@@ -30737,14 +30748,15 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.71"/>
-    <col customWidth="1" min="2" max="2" width="43.29"/>
-    <col customWidth="1" min="3" max="26" width="8.71"/>
+    <col min="1" max="1" customWidth="true" width="17.71"/>
+    <col min="2" max="2" customWidth="true" width="43.29"/>
+    <col min="3" max="26" customWidth="true" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
made changes to excel code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="21936" windowHeight="11460" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="21936" windowHeight="11460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Program" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,11 @@
     <sheet name="Login" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:O40"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>testcase</t>
   </si>
@@ -163,11 +162,18 @@
   <si>
     <t>https://feb-ui-@hackathon.bbfd38d67ea9 herokuapp.com/login</t>
   </si>
+  <si>
+    <t>PFirst</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -258,7 +264,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -267,6 +273,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink 2" xfId="3"/>
@@ -483,12 +490,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" customWidth="1"/>
-    <col min="7" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.88671875"/>
+    <col min="2" max="2" customWidth="true" width="14.33203125"/>
+    <col min="3" max="3" customWidth="true" width="19.5546875"/>
+    <col min="4" max="4" customWidth="true" width="14.6640625"/>
+    <col min="5" max="6" customWidth="true" width="8.88671875"/>
+    <col min="7" max="26" customWidth="true" width="8.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -28523,15 +28530,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="4" width="22.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="7" max="28" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.88671875"/>
+    <col min="2" max="4" customWidth="true" width="22.44140625"/>
+    <col min="5" max="5" customWidth="true" width="14.44140625"/>
+    <col min="6" max="6" customWidth="true" width="17.88671875"/>
+    <col min="7" max="28" customWidth="true" width="8.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1">
@@ -28576,12 +28585,12 @@
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>19</v>
+      <c r="B3" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="4">
-        <v>27</v>
+      <c r="D3" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>17</v>
@@ -29646,7 +29655,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="26" customWidth="true" width="8.6640625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
@@ -30659,15 +30668,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.44140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="57.77734375"/>
+    <col min="3" max="26" customWidth="true" width="8.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
invalid scenarios using scenario outline
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -14,14 +14,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="HmEXYPqxvpRG7s/ayNSWbAN0OTGVt72HvD0buliEC/I="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="Cw4ZH/z7wTBnGnyQXiCXazhJt6Okv3LEIFCuDsxYtOs="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>testcase</t>
   </si>
@@ -80,7 +80,7 @@
     <t>onlyMandatory</t>
   </si>
   <si>
-    <t>javaWebDriver</t>
+    <t>computer</t>
   </si>
   <si>
     <t>invalidBatchNameSuffix</t>
@@ -92,7 +92,19 @@
     <t>invalidBatchNamePrefix</t>
   </si>
   <si>
-    <t>missingOneMandatory</t>
+    <t>missingProgramName</t>
+  </si>
+  <si>
+    <t>missingBatchName</t>
+  </si>
+  <si>
+    <t>missingBatchDescription</t>
+  </si>
+  <si>
+    <t>missingStatus</t>
+  </si>
+  <si>
+    <t>missingNumberOfClasses</t>
   </si>
   <si>
     <t>editAll</t>
@@ -114,7 +126,7 @@
       <rPr>
         <rFont val="Calibri"/>
         <color rgb="FF1155CC"/>
-        <sz val="8.0"/>
+        <sz val="6.0"/>
         <u/>
       </rPr>
       <t>https://jan-ui-hackathon-bbfd38d67ea9.herokuapp.com/login</t>
@@ -128,7 +140,7 @@
       <rPr>
         <rFont val="Calibri"/>
         <color rgb="FF1155CC"/>
-        <sz val="8.0"/>
+        <sz val="6.0"/>
         <u/>
       </rPr>
       <t>https://feb-ui-hackathon-bbfd38d67ea9.herokUuapp.com/login</t>
@@ -144,7 +156,15 @@
     <t>Missing_Protocol</t>
   </si>
   <si>
-    <t>feb-ui-buildathon-bbfd38d67ea99.herokuapp.com/login</t>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF1155CC"/>
+        <sz val="6.0"/>
+        <u/>
+      </rPr>
+      <t>feb-ui-buildathon-bbfd38d67ea99.herokuapp.com/login</t>
+    </r>
   </si>
   <si>
     <t>Incorrect_Endpoint</t>
@@ -154,7 +174,7 @@
       <rPr>
         <rFont val="Calibri"/>
         <color rgb="FF1155CC"/>
-        <sz val="8.0"/>
+        <sz val="6.0"/>
         <u/>
       </rPr>
       <t>https://feb-ui-hackathon-bbfd38d67ea9.herokuapp.com/batch</t>
@@ -168,7 +188,7 @@
       <rPr>
         <rFont val="Calibri"/>
         <color rgb="FF1155CC"/>
-        <sz val="8.0"/>
+        <sz val="6.0"/>
         <u/>
       </rPr>
       <t>https://feb-ui-hackathon-bbfd38d67ea9.herokuapp.com/logginn</t>
@@ -182,7 +202,7 @@
       <rPr>
         <rFont val="Calibri"/>
         <color rgb="FF1155CC"/>
-        <sz val="8.0"/>
+        <sz val="6.0"/>
         <u/>
       </rPr>
       <t>https://feb-ui-hackathon-bbfd38d67ea9.herokuapp.net/login</t>
@@ -196,7 +216,7 @@
       <rPr>
         <rFont val="Calibri"/>
         <color rgb="FF1155CC"/>
-        <sz val="8.0"/>
+        <sz val="6.0"/>
         <u/>
       </rPr>
       <t>https://feb-ui-hackathon-bbfd38d67ea9.herokuapp/</t>
@@ -210,7 +230,7 @@
       <rPr>
         <rFont val="Calibri"/>
         <color rgb="FF1155CC"/>
-        <sz val="8.0"/>
+        <sz val="6.0"/>
         <u/>
       </rPr>
       <t>https://video.feb-ui-hackathon-bbfd38d67ea9.herokuapp.com/login</t>
@@ -223,10 +243,22 @@
     <t>https://feb-ui-@hackathon.bbfd38d67ea9 herokuapp.com/login</t>
   </si>
   <si>
-    <t>70</t>
+    <t>101</t>
   </si>
   <si>
-    <t>71</t>
+    <t>80</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>103</t>
   </si>
 </sst>
 </file>
@@ -262,15 +294,14 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <u/>
-      <sz val="8.0"/>
-      <color rgb="FF0000FF"/>
+      <sz val="6.0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="8.0"/>
-      <color rgb="FF000000"/>
+      <sz val="6.0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -282,7 +313,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border/>
     <border>
       <left style="thin">
@@ -296,6 +327,20 @@
       </top>
       <bottom style="thin">
         <color rgb="FF9A9A9A"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF888888"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF888888"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF888888"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF888888"/>
       </bottom>
     </border>
   </borders>
@@ -325,10 +370,10 @@
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -28603,7 +28648,7 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:F1004"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -28644,8 +28689,8 @@
         <v>16</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="D2" s="4">
-        <v>25.0</v>
+      <c r="D2" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>17</v>
@@ -28663,7 +28708,7 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>17</v>
@@ -28685,6 +28730,9 @@
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="B5" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
@@ -28693,8 +28741,9 @@
       <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
+      <c r="B6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>17</v>
@@ -28707,25 +28756,82 @@
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25" customHeight="1">
+      <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="4">
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25" customHeight="1">
+      <c r="A9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="4">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25" customHeight="1">
+      <c r="A10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="4">
         <v>4.0</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>26</v>
+    <row r="12" ht="14.25" customHeight="1">
+      <c r="A12" s="4" t="s">
+        <v>30</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E12" s="4">
         <v>12312.0</v>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
     <row r="14" ht="14.25" customHeight="1"/>
     <row r="15" ht="14.25" customHeight="1"/>
@@ -29714,6 +29820,10 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -30764,117 +30874,117 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>28</v>
+      <c r="A2" s="8" t="s">
+        <v>32</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>29</v>
+      <c r="B2" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>30</v>
+      <c r="A3" s="8" t="s">
+        <v>34</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>31</v>
+      <c r="B3" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>32</v>
+      <c r="A4" s="8" t="s">
+        <v>36</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>33</v>
+      <c r="B4" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>34</v>
+      <c r="A5" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>36</v>
+      <c r="A6" s="8" t="s">
+        <v>40</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>37</v>
+      <c r="B6" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="6" t="s">
-        <v>38</v>
+      <c r="A7" s="8" t="s">
+        <v>42</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>39</v>
+      <c r="B7" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="6" t="s">
-        <v>40</v>
+      <c r="A8" s="8" t="s">
+        <v>44</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>41</v>
+      <c r="B8" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="6" t="s">
-        <v>42</v>
+      <c r="A9" s="8" t="s">
+        <v>46</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>43</v>
+      <c r="B9" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="6" t="s">
-        <v>44</v>
+      <c r="A10" s="8" t="s">
+        <v>48</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>45</v>
+      <c r="B10" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="6" t="s">
-        <v>46</v>
+      <c r="A11" s="8" t="s">
+        <v>50</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>47</v>
+      <c r="B11" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>

</xml_diff>

<commit_message>
added batch chaining delete scenario in logout
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -2,13 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="Program" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Batch" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Class" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Login" sheetId="4" r:id="rId7"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>testcase</t>
   </si>
@@ -232,11 +234,30 @@
   <si>
     <t>https://feb-ui-@hackathon.bbfd38d67ea9 herokuapp.com/login</t>
   </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="0"/>
   <fonts count="8">
     <font>
       <sz val="11.0"/>
@@ -579,17 +600,18 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.86"/>
-    <col customWidth="1" min="2" max="2" width="14.29"/>
-    <col customWidth="1" min="3" max="3" width="19.57"/>
-    <col customWidth="1" min="4" max="4" width="14.71"/>
-    <col customWidth="1" min="5" max="6" width="8.86"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" customWidth="true" width="14.86"/>
+    <col min="2" max="2" customWidth="true" width="14.29"/>
+    <col min="3" max="3" customWidth="true" width="19.57"/>
+    <col min="4" max="4" customWidth="true" width="14.71"/>
+    <col min="5" max="6" customWidth="true" width="8.86"/>
+    <col min="7" max="26" customWidth="true" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -28627,16 +28649,17 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F1004"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.86"/>
-    <col customWidth="1" min="2" max="4" width="22.43"/>
-    <col customWidth="1" min="5" max="5" width="14.43"/>
-    <col customWidth="1" min="6" max="6" width="17.86"/>
-    <col customWidth="1" min="7" max="28" width="8.71"/>
+    <col min="1" max="1" customWidth="true" width="23.86"/>
+    <col min="2" max="4" customWidth="true" width="22.43"/>
+    <col min="5" max="5" customWidth="true" width="14.43"/>
+    <col min="6" max="6" customWidth="true" width="17.86"/>
+    <col min="7" max="28" customWidth="true" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -28667,8 +28690,8 @@
         <v>16</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="D2" s="4">
-        <v>25.0</v>
+      <c r="D2" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>17</v>
@@ -28685,8 +28708,8 @@
         <v>19</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="4">
-        <v>80.0</v>
+      <c r="D3" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>17</v>
@@ -28720,8 +28743,8 @@
         <v>23</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="D6" s="4">
-        <v>100.0</v>
+      <c r="D6" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>17</v>
@@ -28751,8 +28774,8 @@
       <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4">
-        <v>100.0</v>
+      <c r="D8" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4">
@@ -28783,8 +28806,8 @@
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="4">
-        <v>100.0</v>
+      <c r="D10" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>17</v>
@@ -29820,7 +29843,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col min="1" max="26" customWidth="true" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
@@ -30836,14 +30859,15 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.71"/>
-    <col customWidth="1" min="2" max="2" width="43.29"/>
-    <col customWidth="1" min="3" max="26" width="8.71"/>
+    <col min="1" max="1" customWidth="true" width="17.71"/>
+    <col min="2" max="2" customWidth="true" width="43.29"/>
+    <col min="3" max="26" customWidth="true" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">

</xml_diff>